<commit_message>
minor updates for FGI paper
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_glucose_Acrylic_300L_FGI.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_glucose_Acrylic_300L_FGI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\acrylic_acid_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC619D1C-59BE-426A-9E83-905F911F8721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DA87E8-B772-4952-9376-D11B7C181FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>